<commit_message>
new results for step 1
</commit_message>
<xml_diff>
--- a/preprocessingData/resultsAlgoGenetiqueCalculs.xlsx
+++ b/preprocessingData/resultsAlgoGenetiqueCalculs.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="resultsAlgoGenetique" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>nbChr50-nbStep10</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t>nbChr10000-nbStep100</t>
   </si>
 </sst>
 </file>
@@ -919,18 +922,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -949,8 +952,11 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -972,28 +978,39 @@
       <c r="H2">
         <v>1.8223315509299998E-2</v>
       </c>
-      <c r="J2" s="2" t="str">
+      <c r="I2">
+        <v>2.19137451956E-2</v>
+      </c>
+      <c r="K2" s="2" t="str">
         <f>A2</f>
         <v>A</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="3">
-        <f>AVERAGE(F2:H2)</f>
-        <v>1.8673510937166665E-2</v>
-      </c>
-      <c r="M2" s="1"/>
-      <c r="N2">
+      <c r="M2" s="3">
+        <f>AVERAGE(F2:I2)</f>
+        <v>1.9483569501774996E-2</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2">
         <f>100*_xlfn.VAR.P(F2:H2)/AVERAGE(F2:H2)</f>
         <v>9.4417235667649813E-2</v>
       </c>
-      <c r="O2">
-        <f>LOG10(ABS(N2))</f>
+      <c r="P2">
+        <f>LOG10(ABS(O2))</f>
         <v>-1.0249487189212878</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <f>100*_xlfn.VAR.P(F2:I2)/AVERAGE(F2:I2)</f>
+        <v>7.7972592520219097E-2</v>
+      </c>
+      <c r="R2">
+        <f>LOG10(ABS(Q2))</f>
+        <v>-1.1080580256291737</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1015,28 +1032,39 @@
       <c r="H3">
         <v>2.6934247600000001</v>
       </c>
-      <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J23" si="0">A3</f>
+      <c r="I3">
+        <v>1.3350910090799999</v>
+      </c>
+      <c r="K3" s="2" t="str">
+        <f t="shared" ref="K3:K23" si="0">A3</f>
         <v>B</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="3">
-        <f t="shared" ref="L3:L23" si="1">AVERAGE(F3:H3)</f>
-        <v>2.5308534487166665</v>
-      </c>
-      <c r="M3" s="1"/>
-      <c r="N3">
-        <f t="shared" ref="N3:N23" si="2">100*_xlfn.VAR.P(F3:H3)/AVERAGE(F3:H3)</f>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M23" si="1">AVERAGE(F3:I3)</f>
+        <v>2.2319128388074998</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3">
+        <f>100*_xlfn.VAR.P(F3:H3)/AVERAGE(F3:H3)</f>
         <v>1.9087783194926546</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O23" si="3">LOG10(ABS(N3))</f>
+      <c r="P3">
+        <f t="shared" ref="P3:P23" si="2">LOG10(ABS(O3))</f>
         <v>0.28075549350031415</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <f>100*_xlfn.VAR.P(F3:I3)/AVERAGE(F3:I3)</f>
+        <v>13.635288346054871</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R23" si="3">LOG10(ABS(Q3))</f>
+        <v>1.1346643264196661</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1058,28 +1086,39 @@
       <c r="H4">
         <v>8.87258730612E-2</v>
       </c>
-      <c r="J4" s="2" t="str">
+      <c r="I4">
+        <v>7.4885153642400004E-2</v>
+      </c>
+      <c r="K4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <f t="shared" si="1"/>
-        <v>5.8163577588666665E-2</v>
-      </c>
-      <c r="M4" s="1"/>
-      <c r="N4">
+        <v>6.23439716021E-2</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4">
+        <f>100*_xlfn.VAR.P(F4:H4)/AVERAGE(F4:H4)</f>
+        <v>1.2085820480690292</v>
+      </c>
+      <c r="P4">
         <f t="shared" si="2"/>
-        <v>1.2085820480690292</v>
-      </c>
-      <c r="O4">
+        <v>8.2276139074722282E-2</v>
+      </c>
+      <c r="Q4">
+        <f>100*_xlfn.VAR.P(F4:I4)/AVERAGE(F4:I4)</f>
+        <v>0.92974987856182367</v>
+      </c>
+      <c r="R4">
         <f t="shared" si="3"/>
-        <v>8.2276139074722282E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>-3.163386969384413E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1101,28 +1140,39 @@
       <c r="H5">
         <v>-0.27753725190299999</v>
       </c>
-      <c r="J5" s="2" t="str">
+      <c r="I5">
+        <v>0.51866724853000001</v>
+      </c>
+      <c r="K5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <f t="shared" si="1"/>
-        <v>-0.35776839478033334</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5">
+        <v>-0.13865948395274999</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5">
+        <f>100*_xlfn.VAR.P(F5:H5)/AVERAGE(F5:H5)</f>
+        <v>-9.0869216829303436</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="2"/>
-        <v>-9.0869216829303436</v>
-      </c>
-      <c r="O5">
+        <v>0.95841678503306604</v>
+      </c>
+      <c r="Q5">
+        <f>100*_xlfn.VAR.P(F5:I5)/AVERAGE(F5:I5)</f>
+        <v>-121.45490520468944</v>
+      </c>
+      <c r="R5">
         <f t="shared" si="3"/>
-        <v>0.95841678503306604</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2.0844150593660182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1144,28 +1194,39 @@
       <c r="H6">
         <v>1.1598088252300001</v>
       </c>
-      <c r="J6" s="2" t="str">
+      <c r="I6">
+        <v>0.34489748755499999</v>
+      </c>
+      <c r="K6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="3">
         <f t="shared" si="1"/>
-        <v>1.6657392331373335</v>
-      </c>
-      <c r="M6" s="1"/>
-      <c r="N6">
+        <v>1.3355287967417502</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6">
+        <f>100*_xlfn.VAR.P(F6:H6)/AVERAGE(F6:H6)</f>
+        <v>49.851901977147506</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="2"/>
-        <v>49.851901977147506</v>
-      </c>
-      <c r="O6">
+        <v>1.6976817324053941</v>
+      </c>
+      <c r="Q6">
+        <f>100*_xlfn.VAR.P(F6:I6)/AVERAGE(F6:I6)</f>
+        <v>71.12679385911089</v>
+      </c>
+      <c r="R6">
         <f t="shared" si="3"/>
-        <v>1.6976817324053941</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.8520332327006865</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1187,28 +1248,39 @@
       <c r="H7">
         <v>1.97334612853</v>
       </c>
-      <c r="J7" s="2" t="str">
+      <c r="I7">
+        <v>0.898849743476</v>
+      </c>
+      <c r="K7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <f t="shared" si="1"/>
-        <v>1.5015208511133336</v>
-      </c>
-      <c r="M7" s="1"/>
-      <c r="N7">
+        <v>1.3508530742040001</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7">
+        <f>100*_xlfn.VAR.P(F7:H7)/AVERAGE(F7:H7)</f>
+        <v>21.521102586990679</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="2"/>
-        <v>21.521102586990679</v>
-      </c>
-      <c r="O7">
+        <v>1.3328645176997096</v>
+      </c>
+      <c r="Q7">
+        <f>100*_xlfn.VAR.P(F7:I7)/AVERAGE(F7:I7)</f>
+        <v>22.982530445008575</v>
+      </c>
+      <c r="R7">
         <f t="shared" si="3"/>
-        <v>1.3328645176997096</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.3613978440999805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1230,28 +1302,39 @@
       <c r="H8">
         <v>0.59729593385400004</v>
       </c>
-      <c r="J8" s="2" t="str">
+      <c r="I8">
+        <v>0.26923137637200001</v>
+      </c>
+      <c r="K8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>G</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <f t="shared" si="1"/>
-        <v>0.52030993602466669</v>
-      </c>
-      <c r="M8" s="1"/>
-      <c r="N8">
+        <v>0.45754029611149999</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8">
+        <f>100*_xlfn.VAR.P(F8:H8)/AVERAGE(F8:H8)</f>
+        <v>6.4000501570699431</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="2"/>
-        <v>6.4000501570699431</v>
-      </c>
-      <c r="O8">
+        <v>0.8061833775547228</v>
+      </c>
+      <c r="Q8">
+        <f>100*_xlfn.VAR.P(F8:I8)/AVERAGE(F8:I8)</f>
+        <v>8.0419486667174187</v>
+      </c>
+      <c r="R8">
         <f t="shared" si="3"/>
-        <v>0.8061833775547228</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.90536129659174736</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1273,28 +1356,39 @@
       <c r="H9">
         <v>0.41520729237600001</v>
       </c>
-      <c r="J9" s="2" t="str">
+      <c r="I9">
+        <v>0.71902405272199998</v>
+      </c>
+      <c r="K9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>H</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <f t="shared" si="1"/>
-        <v>0.54352528774966669</v>
-      </c>
-      <c r="M9" s="1"/>
-      <c r="N9">
+        <v>0.58739997899274998</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9">
+        <f>100*_xlfn.VAR.P(F9:H9)/AVERAGE(F9:H9)</f>
+        <v>7.8677405723934219</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="2"/>
-        <v>7.8677405723934219</v>
-      </c>
-      <c r="O9">
+        <v>0.8958500312377029</v>
+      </c>
+      <c r="Q9">
+        <f>100*_xlfn.VAR.P(F9:I9)/AVERAGE(F9:I9)</f>
+        <v>6.4431965675332137</v>
+      </c>
+      <c r="R9">
         <f t="shared" si="3"/>
-        <v>0.8958500312377029</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.80910138090288608</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1316,28 +1410,39 @@
       <c r="H10">
         <v>1.24511367251</v>
       </c>
-      <c r="J10" s="2" t="str">
+      <c r="I10">
+        <v>1.6367103921499999</v>
+      </c>
+      <c r="K10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>I-1</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="3">
+      <c r="M10" s="3">
         <f t="shared" si="1"/>
-        <v>2.5088764469766667</v>
-      </c>
-      <c r="M10" s="1"/>
-      <c r="N10">
+        <v>2.2908349332700002</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10">
+        <f>100*_xlfn.VAR.P(F10:H10)/AVERAGE(F10:H10)</f>
+        <v>107.89290547233009</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="2"/>
-        <v>107.89290547233009</v>
-      </c>
-      <c r="O10">
+        <v>2.0329928884686725</v>
+      </c>
+      <c r="Q10">
+        <f>100*_xlfn.VAR.P(F10:I10)/AVERAGE(F10:I10)</f>
+        <v>94.84756162734665</v>
+      </c>
+      <c r="R10">
         <f t="shared" si="3"/>
-        <v>2.0329928884686725</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.9770261703812417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1359,28 +1464,39 @@
       <c r="H11">
         <v>-0.97938994046399996</v>
       </c>
-      <c r="J11" s="2" t="str">
+      <c r="I11">
+        <v>6.0658794578300002E-3</v>
+      </c>
+      <c r="K11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>I-2</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11" s="3">
         <f t="shared" si="1"/>
-        <v>-0.83155439185299995</v>
-      </c>
-      <c r="M11" s="1"/>
-      <c r="N11">
+        <v>-0.62214932402529244</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11">
+        <f>100*_xlfn.VAR.P(F11:H11)/AVERAGE(F11:H11)</f>
+        <v>-2.7292879343274539</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="2"/>
-        <v>-2.7292879343274539</v>
-      </c>
-      <c r="O11">
+        <v>0.43604935527164135</v>
+      </c>
+      <c r="Q11">
+        <f>100*_xlfn.VAR.P(F11:I11)/AVERAGE(F11:I11)</f>
+        <v>-23.880614640497594</v>
+      </c>
+      <c r="R11">
         <f t="shared" si="3"/>
-        <v>0.43604935527164135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.3780455004950718</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1402,28 +1518,39 @@
       <c r="H12">
         <v>4.7938164222099999</v>
       </c>
-      <c r="J12" s="2" t="str">
+      <c r="I12">
+        <v>3.3381221070499998</v>
+      </c>
+      <c r="K12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>I0</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="3">
+      <c r="M12" s="3">
         <f t="shared" si="1"/>
-        <v>4.1474361925899998</v>
-      </c>
-      <c r="M12" s="1"/>
-      <c r="N12">
+        <v>3.9451076712049997</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12">
+        <f>100*_xlfn.VAR.P(F12:H12)/AVERAGE(F12:H12)</f>
+        <v>5.0387174942300161</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="2"/>
-        <v>5.0387174942300161</v>
-      </c>
-      <c r="O12">
+        <v>0.70232000944995499</v>
+      </c>
+      <c r="Q12">
+        <f>100*_xlfn.VAR.P(F12:I12)/AVERAGE(F12:I12)</f>
+        <v>7.0858316107930781</v>
+      </c>
+      <c r="R12">
         <f t="shared" si="3"/>
-        <v>0.70232000944995499</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.8503908274535068</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1445,28 +1572,39 @@
       <c r="H13">
         <v>4.7393219254299996</v>
       </c>
-      <c r="J13" s="2" t="str">
+      <c r="I13">
+        <v>2.7815407906399998</v>
+      </c>
+      <c r="K13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>I1</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13" s="3">
         <f t="shared" si="1"/>
-        <v>4.582011311423333</v>
-      </c>
-      <c r="M13" s="1"/>
-      <c r="N13">
+        <v>4.1318936812275</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13">
+        <f>100*_xlfn.VAR.P(F13:H13)/AVERAGE(F13:H13)</f>
+        <v>2.0361947259949438</v>
+      </c>
+      <c r="P13">
         <f t="shared" si="2"/>
-        <v>2.0361947259949438</v>
-      </c>
-      <c r="O13">
+        <v>0.30881930823310111</v>
+      </c>
+      <c r="Q13">
+        <f>100*_xlfn.VAR.P(F13:I13)/AVERAGE(F13:I13)</f>
+        <v>16.403898547039816</v>
+      </c>
+      <c r="R13">
         <f t="shared" si="3"/>
-        <v>0.30881930823310111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.2149470746487907</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1488,28 +1626,39 @@
       <c r="H14">
         <v>2.8966878017700002</v>
       </c>
-      <c r="J14" s="2" t="str">
+      <c r="I14">
+        <v>0.79483266022400001</v>
+      </c>
+      <c r="K14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>I2</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <f t="shared" si="1"/>
-        <v>2.41527346642</v>
-      </c>
-      <c r="M14" s="1"/>
-      <c r="N14">
+        <v>2.0101632648709997</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14">
+        <f>100*_xlfn.VAR.P(F14:H14)/AVERAGE(F14:H14)</f>
+        <v>12.022362755370958</v>
+      </c>
+      <c r="P14">
         <f t="shared" si="2"/>
-        <v>12.022362755370958</v>
-      </c>
-      <c r="O14">
+        <v>1.0799898279645781</v>
+      </c>
+      <c r="Q14">
+        <f>100*_xlfn.VAR.P(F14:I14)/AVERAGE(F14:I14)</f>
+        <v>35.326609627064897</v>
+      </c>
+      <c r="R14">
         <f t="shared" si="3"/>
-        <v>1.0799898279645781</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.5481019592318801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1531,28 +1680,39 @@
       <c r="H15">
         <v>1.1420627687</v>
       </c>
-      <c r="J15" s="2" t="str">
+      <c r="I15">
+        <v>1.07462531438</v>
+      </c>
+      <c r="K15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>I3</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L15" s="3">
+      <c r="M15" s="3">
         <f t="shared" si="1"/>
-        <v>1.0007839034786665</v>
-      </c>
-      <c r="M15" s="1"/>
-      <c r="N15">
+        <v>1.0192442562039998</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15">
+        <f>100*_xlfn.VAR.P(F15:H15)/AVERAGE(F15:H15)</f>
+        <v>1.4696235971526024</v>
+      </c>
+      <c r="P15">
         <f t="shared" si="2"/>
-        <v>1.4696235971526024</v>
-      </c>
-      <c r="O15">
+        <v>0.16720611664484533</v>
+      </c>
+      <c r="Q15">
+        <f>100*_xlfn.VAR.P(F15:I15)/AVERAGE(F15:I15)</f>
+        <v>1.182559636356624</v>
+      </c>
+      <c r="R15">
         <f t="shared" si="3"/>
-        <v>0.16720611664484533</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7.2823051386619625E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1574,28 +1734,39 @@
       <c r="H16">
         <v>1.1201975958799999</v>
       </c>
-      <c r="J16" s="2" t="str">
+      <c r="I16">
+        <v>2.8755985419200001</v>
+      </c>
+      <c r="K16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>I4</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="3">
+      <c r="M16" s="3">
         <f t="shared" si="1"/>
-        <v>1.0372565278970001</v>
-      </c>
-      <c r="M16" s="1"/>
-      <c r="N16">
+        <v>1.4968420314027502</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16">
+        <f>100*_xlfn.VAR.P(F16:H16)/AVERAGE(F16:H16)</f>
+        <v>0.85759623057742373</v>
+      </c>
+      <c r="P16">
         <f t="shared" si="2"/>
-        <v>0.85759623057742373</v>
-      </c>
-      <c r="O16">
+        <v>-6.6717136516769859E-2</v>
+      </c>
+      <c r="Q16">
+        <f>100*_xlfn.VAR.P(F16:I16)/AVERAGE(F16:I16)</f>
+        <v>42.778602973977222</v>
+      </c>
+      <c r="R16">
         <f t="shared" si="3"/>
-        <v>-6.6717136516769859E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.6312265976595499</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1617,28 +1788,39 @@
       <c r="H17">
         <v>0.61824987509600005</v>
       </c>
-      <c r="J17" s="2" t="str">
+      <c r="I17">
+        <v>1.4616523876500001</v>
+      </c>
+      <c r="K17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>J</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L17" s="3">
+      <c r="M17" s="3">
         <f t="shared" si="1"/>
-        <v>0.41519818459353336</v>
-      </c>
-      <c r="M17" s="1"/>
-      <c r="N17">
+        <v>0.67681173535765005</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17">
+        <f>100*_xlfn.VAR.P(F17:H17)/AVERAGE(F17:H17)</f>
+        <v>18.879002775120725</v>
+      </c>
+      <c r="P17">
         <f t="shared" si="2"/>
-        <v>18.879002775120725</v>
-      </c>
-      <c r="O17">
+        <v>1.2759790503063095</v>
+      </c>
+      <c r="Q17">
+        <f>100*_xlfn.VAR.P(F17:I17)/AVERAGE(F17:I17)</f>
+        <v>39.023245849070342</v>
+      </c>
+      <c r="R17">
         <f t="shared" si="3"/>
-        <v>1.2759790503063095</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.5913233900127042</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1660,28 +1842,39 @@
       <c r="H18">
         <v>2.8046727434599998</v>
       </c>
-      <c r="J18" s="2" t="str">
+      <c r="I18">
+        <v>1.1693170335600001</v>
+      </c>
+      <c r="K18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>K0</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="L18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L18" s="3">
+      <c r="M18" s="3">
         <f t="shared" si="1"/>
-        <v>1.3314151885266667</v>
-      </c>
-      <c r="M18" s="1"/>
-      <c r="N18">
+        <v>1.2908906497850001</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18">
+        <f>100*_xlfn.VAR.P(F18:H18)/AVERAGE(F18:H18)</f>
+        <v>175.65453561197845</v>
+      </c>
+      <c r="P18">
         <f t="shared" si="2"/>
-        <v>175.65453561197845</v>
-      </c>
-      <c r="O18">
+        <v>2.2446593682801814</v>
+      </c>
+      <c r="Q18">
+        <f>100*_xlfn.VAR.P(F18:I18)/AVERAGE(F18:I18)</f>
+        <v>136.25825625656415</v>
+      </c>
+      <c r="R18">
         <f t="shared" si="3"/>
-        <v>2.2446593682801814</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2.1343628268241499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1703,28 +1896,39 @@
       <c r="H19">
         <v>0.349995966253</v>
       </c>
-      <c r="J19" s="2" t="str">
+      <c r="I19">
+        <v>1.3151755044</v>
+      </c>
+      <c r="K19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>K1</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L19" s="3">
+      <c r="M19" s="3">
         <f t="shared" si="1"/>
-        <v>-1.9689057470899995E-2</v>
-      </c>
-      <c r="M19" s="1"/>
-      <c r="N19">
+        <v>0.31402708299682502</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19">
+        <f>100*_xlfn.VAR.P(F19:H19)/AVERAGE(F19:H19)</f>
+        <v>-419.79964708199412</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="2"/>
-        <v>-419.79964708199412</v>
-      </c>
-      <c r="O19">
+        <v>2.6230420691429823</v>
+      </c>
+      <c r="Q19">
+        <f>100*_xlfn.VAR.P(F19:I19)/AVERAGE(F19:I19)</f>
+        <v>126.13253888120364</v>
+      </c>
+      <c r="R19">
         <f t="shared" si="3"/>
-        <v>2.6230420691429823</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2.1008271375931056</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1746,28 +1950,39 @@
       <c r="H20">
         <v>2.1114371060599999</v>
       </c>
-      <c r="J20" s="2" t="str">
+      <c r="I20">
+        <v>1.3440063666099999</v>
+      </c>
+      <c r="K20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>K2</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L20" s="3">
+      <c r="M20" s="3">
         <f t="shared" si="1"/>
-        <v>1.5880900939723332</v>
-      </c>
-      <c r="M20" s="1"/>
-      <c r="N20">
+        <v>1.5270691621317498</v>
+      </c>
+      <c r="N20" s="1"/>
+      <c r="O20">
+        <f>100*_xlfn.VAR.P(F20:H20)/AVERAGE(F20:H20)</f>
+        <v>18.711938224931789</v>
+      </c>
+      <c r="P20">
         <f t="shared" si="2"/>
-        <v>18.711938224931789</v>
-      </c>
-      <c r="O20">
+        <v>1.2721187750358376</v>
+      </c>
+      <c r="Q20">
+        <f>100*_xlfn.VAR.P(F20:I20)/AVERAGE(F20:I20)</f>
+        <v>15.326253464946886</v>
+      </c>
+      <c r="R20">
         <f t="shared" si="3"/>
-        <v>1.2721187750358376</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.1854360036242657</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1789,28 +2004,39 @@
       <c r="H21">
         <v>-0.36735076586999998</v>
       </c>
-      <c r="J21" s="2" t="str">
+      <c r="I21">
+        <v>1.6553731645500001</v>
+      </c>
+      <c r="K21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>L</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L21" s="3">
+      <c r="M21" s="3">
         <f t="shared" si="1"/>
-        <v>-7.3334484433000002E-2</v>
-      </c>
-      <c r="M21" s="1"/>
-      <c r="N21">
+        <v>0.35884242781275</v>
+      </c>
+      <c r="N21" s="1"/>
+      <c r="O21">
+        <f>100*_xlfn.VAR.P(F21:H21)/AVERAGE(F21:H21)</f>
+        <v>-732.52704784953551</v>
+      </c>
+      <c r="P21">
         <f t="shared" si="2"/>
-        <v>-732.52704784953551</v>
-      </c>
-      <c r="O21">
+        <v>2.8648236652240033</v>
+      </c>
+      <c r="Q21">
+        <f>100*_xlfn.VAR.P(F21:I21)/AVERAGE(F21:I21)</f>
+        <v>268.42613252577519</v>
+      </c>
+      <c r="R21">
         <f t="shared" si="3"/>
-        <v>2.8648236652240033</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2.4288247941321082</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1832,28 +2058,39 @@
       <c r="H22">
         <v>0.39904522651199997</v>
       </c>
-      <c r="J22" s="2" t="str">
+      <c r="I22">
+        <v>1.3593467557000001</v>
+      </c>
+      <c r="K22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>M</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="3">
+      <c r="M22" s="3">
         <f t="shared" si="1"/>
-        <v>0.7551804202893333</v>
-      </c>
-      <c r="M22" s="1"/>
-      <c r="N22">
+        <v>0.90622200414199994</v>
+      </c>
+      <c r="N22" s="1"/>
+      <c r="O22">
+        <f>100*_xlfn.VAR.P(F22:H22)/AVERAGE(F22:H22)</f>
+        <v>315.93190139638625</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="2"/>
-        <v>315.93190139638625</v>
-      </c>
-      <c r="O22">
+        <v>2.4995934812419773</v>
+      </c>
+      <c r="Q22">
+        <f>100*_xlfn.VAR.P(F22:I22)/AVERAGE(F22:I22)</f>
+        <v>205.00854837575079</v>
+      </c>
+      <c r="R22">
         <f t="shared" si="3"/>
-        <v>2.4995934812419773</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2.3117719704948527</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1875,29 +2112,52 @@
       <c r="H23">
         <v>4.6727935269999996</v>
       </c>
-      <c r="J23" s="2" t="str">
+      <c r="I23">
+        <v>4.3829249492600004</v>
+      </c>
+      <c r="K23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>N</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L23" s="3">
+      <c r="M23" s="3">
         <f t="shared" si="1"/>
-        <v>3.7813005509533331</v>
-      </c>
-      <c r="M23" s="1"/>
-      <c r="N23">
+        <v>3.9317066505299998</v>
+      </c>
+      <c r="N23" s="1"/>
+      <c r="O23">
+        <f>100*_xlfn.VAR.P(F23:H23)/AVERAGE(F23:H23)</f>
+        <v>10.509337268669556</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="2"/>
-        <v>10.509337268669556</v>
-      </c>
-      <c r="O23">
+        <v>1.0215753297642309</v>
+      </c>
+      <c r="Q23">
+        <f>100*_xlfn.VAR.P(F23:I23)/AVERAGE(F23:I23)</f>
+        <v>9.3065998540757047</v>
+      </c>
+      <c r="R23">
         <f t="shared" si="3"/>
-        <v>1.0215753297642309</v>
+        <v>0.96879104141873917</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O2:O23">
+  <conditionalFormatting sqref="R2:R23">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P23">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>